<commit_message>
Gestione: aggiornato file ore
</commit_message>
<xml_diff>
--- a/Ore dedicate.xlsx
+++ b/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B9FA2-39FD-4E6A-A41A-795F4D6BAFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BC9966-B82F-4875-A67F-0DEE2DB8A150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Data</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Funghi</t>
+  </si>
+  <si>
+    <t>Scritti testi primi quattro funghi</t>
+  </si>
+  <si>
+    <t>Creata struttura gestione funghi etc</t>
   </si>
 </sst>
 </file>
@@ -85,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -166,9 +172,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -452,7 +458,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,22 +533,34 @@
         <v>45645</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="7">
         <f>SUM(D:D)</f>
-        <v>0.20833333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D5" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione: pulizia e aggiornamento note, appunti etc
</commit_message>
<xml_diff>
--- a/Ore dedicate.xlsx
+++ b/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0218070-3891-45BD-B3B9-FB648EDC237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE601432-C841-461E-8A50-F2249D1568FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Data</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Costruzione palette, reference</t>
+  </si>
+  <si>
+    <t>Ink - Generale</t>
+  </si>
+  <si>
+    <t>Ora la struttura ragiona partendo da "main"</t>
+  </si>
+  <si>
+    <t>Sistemati piccoli bug e simili</t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +564,7 @@
       </c>
       <c r="F4" s="7">
         <f>SUM(D:D)</f>
-        <v>0.55208333333333337</v>
+        <v>0.67708333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -587,6 +596,28 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>45647</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione: appunti vari, cose da fare e come
</commit_message>
<xml_diff>
--- a/Ore dedicate.xlsx
+++ b/Ore dedicate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE601432-C841-461E-8A50-F2249D1568FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CAC040-415F-4D4F-AE00-AA27332D528C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Data</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Sistemati piccoli bug e simili</t>
+  </si>
+  <si>
+    <t>Gestione</t>
+  </si>
+  <si>
+    <t>Appunti e cose varie</t>
   </si>
 </sst>
 </file>
@@ -473,23 +479,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="49.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -509,7 +515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45637</v>
       </c>
@@ -526,7 +532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45637</v>
       </c>
@@ -546,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45645</v>
       </c>
@@ -564,10 +570,10 @@
       </c>
       <c r="F4" s="7">
         <f>SUM(D:D)</f>
-        <v>0.67708333333333337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -581,7 +587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45646</v>
       </c>
@@ -598,7 +604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45647</v>
       </c>
@@ -615,9 +621,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>